<commit_message>
working on parser, finished base class schedule creator, added skills.md
</commit_message>
<xml_diff>
--- a/output/sample_schedule.xlsx
+++ b/output/sample_schedule.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Region 8 Schedule" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Region 8" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -523,10 +523,10 @@
       </c>
       <c r="I1" s="4" t="n"/>
       <c r="J1" s="5" t="n">
-        <v>46068.98641715629</v>
+        <v>46068.03690673139</v>
       </c>
       <c r="K1" s="5" t="n">
-        <v>46074.98641715629</v>
+        <v>46074.03690673139</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">

</xml_diff>